<commit_message>
change to the databases
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>username</t>
   </si>
@@ -44,9 +44,6 @@
     <t>type</t>
   </si>
   <si>
-    <t>student table</t>
-  </si>
-  <si>
     <t>exam</t>
   </si>
   <si>
@@ -69,6 +66,48 @@
   </si>
   <si>
     <t>admin</t>
+  </si>
+  <si>
+    <t>preference</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">username id </t>
+  </si>
+  <si>
+    <t>exams table</t>
+  </si>
+  <si>
+    <t>exam id</t>
+  </si>
+  <si>
+    <t>exam name</t>
+  </si>
+  <si>
+    <t>qualification id</t>
+  </si>
+  <si>
+    <t>qualification name</t>
+  </si>
+  <si>
+    <t>request tables</t>
+  </si>
+  <si>
+    <t>response table</t>
+  </si>
+  <si>
+    <t>request id</t>
+  </si>
+  <si>
+    <t>reqid</t>
+  </si>
+  <si>
+    <t>vol id</t>
+  </si>
+  <si>
+    <t>date</t>
   </si>
 </sst>
 </file>
@@ -420,115 +459,153 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A25"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="E10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="E11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="E16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="E17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="E19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>1</v>
       </c>

</xml_diff>